<commit_message>
Ok, je lui laisse une chance
</commit_message>
<xml_diff>
--- a/inst/extdata/ECKMUHL_matrice.xlsx
+++ b/inst/extdata/ECKMUHL_matrice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phgourmain-my.sharepoint.com/personal/p_carteron_racines_com/Documents/personnel/Rsequoia2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_A23FF25D330BFBBDAE164C627148F66B06B9EA07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68871B52-FBAD-459C-BA5D-0B7FF90736DA}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_A23FF25D330BFBBDAE164C627148F66B06B9EA07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB203AED-E8BF-4C7E-B4D3-BBA9F423BE3A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21285" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRICE" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,7 +150,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +487,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -497,7 +496,7 @@
     <col min="2" max="2" width="18.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.9453125" customWidth="1"/>
     <col min="7" max="7" width="17.68359375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
@@ -544,7 +543,7 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2">
         <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -570,7 +569,7 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3">
         <v>697</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -596,7 +595,7 @@
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4">
         <v>698</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -622,7 +621,7 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5">
         <v>699</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -648,7 +647,7 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>700</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -674,7 +673,7 @@
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
         <v>701</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -700,7 +699,7 @@
       <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
         <v>702</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -726,7 +725,7 @@
       <c r="E9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9">
         <v>703</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -752,7 +751,7 @@
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10">
         <v>704</v>
       </c>
       <c r="G10" s="2" t="s">

</xml_diff>

<commit_message>
skip ua_to_ua if qgis isn't installed
</commit_message>
<xml_diff>
--- a/inst/extdata/ECKMUHL_matrice.xlsx
+++ b/inst/extdata/ECKMUHL_matrice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phgourmain-my.sharepoint.com/personal/p_carteron_racines_com/Documents/personnel/Rsequoia2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_A23FF25D330BFBBDAE164C627148F66B06B9EA07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB203AED-E8BF-4C7E-B4D3-BBA9F423BE3A}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_A23FF25D330BFBBDAE164C627148F66B06B9EA07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{687F0A88-EDE9-40C3-9C06-53E22E706A06}"/>
   <bookViews>
-    <workbookView xWindow="21285" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATRICE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
   <si>
     <t>IDENTIFIANT</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>LIEU_DIT</t>
-  </si>
-  <si>
-    <t>TX_BOISEE</t>
   </si>
   <si>
     <t>000</t>
@@ -94,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,20 +117,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,13 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -484,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -498,10 +480,9 @@
     <col min="4" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.9453125" customWidth="1"/>
     <col min="7" max="7" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,242 +504,212 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2">
         <v>29158</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>29158</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>697</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>29158</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>698</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <v>29158</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>699</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <v>29158</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>700</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>29158</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>701</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>29158</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>702</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>29158</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>703</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
         <v>29158</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>704</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add id in filename capability to #22
</commit_message>
<xml_diff>
--- a/inst/extdata/ECKMUHL_matrice.xlsx
+++ b/inst/extdata/ECKMUHL_matrice.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phgourmain-my.sharepoint.com/personal/p_carteron_racines_com/Documents/personnel/Rsequoia2/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_A23FF25D330BFBBDAE164C627148F66B06B9EA07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A645B34E-CEE5-4D29-B09B-24C53313565A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_6028B9AD3215917CA24FA4A37C4D9EAD87B3D500" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCDBCC7-34D1-4D24-85E0-6EFE80139331}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MATRICE" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,62 +22,50 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
   <si>
+    <t>PROPRIETAIRE</t>
+  </si>
+  <si>
+    <t>INSEE</t>
+  </si>
+  <si>
+    <t>PREFIXE</t>
+  </si>
+  <si>
+    <t>SECTION</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>LIEU_DIT</t>
+  </si>
+  <si>
+    <t>PEMNARCH</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>PHARE D ECKMUHL</t>
+  </si>
+  <si>
     <t>IDENTIFIANT</t>
   </si>
   <si>
-    <t>PROPRIETAIRE</t>
-  </si>
-  <si>
-    <t>INSEE</t>
-  </si>
-  <si>
-    <t>PREFIXE</t>
-  </si>
-  <si>
-    <t>SECTION</t>
-  </si>
-  <si>
-    <t>NUMERO</t>
-  </si>
-  <si>
-    <t>LIEU_DIT</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>ECKMUHL</t>
-  </si>
-  <si>
-    <t>PEMNARCH</t>
-  </si>
-  <si>
-    <t>AX</t>
-  </si>
-  <si>
-    <t>PHARE D ECKMUHL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,39 +87,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,253 +430,242 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="12.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.9453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.26171875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="2"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>29158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
         <v>696</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>29158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
         <v>697</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>29158</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
         <v>698</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
+      <c r="G4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>29158</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
         <v>699</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
+      <c r="G5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>29158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
         <v>700</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>11</v>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>29158</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
         <v>701</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
+      <c r="G7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>29158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
         <v>702</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
+      <c r="G8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>29158</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
         <v>703</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>11</v>
+      <c r="G9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2">
-        <v>29158</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>29158</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10">
         <v>704</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>11</v>
+      <c r="G10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>